<commit_message>
feat: add akiApcMni Mapping
</commit_message>
<xml_diff>
--- a/mappings/AKAI_APC_mini/Keypad.xlsx
+++ b/mappings/AKAI_APC_mini/Keypad.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pascal\Documents\GitHub\pam-osc\mappings\AKAI_APC_mini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E52D462-4997-48DF-B62D-446ED1ED5E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9AAC69-2841-4D7C-9673-6E40EC517EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" xr2:uid="{17A9B8A9-425F-4B9B-A662-A90AFB771B06}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="24220" windowHeight="15500" activeTab="1" xr2:uid="{17A9B8A9-425F-4B9B-A662-A90AFB771B06}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="akiApcMini1" sheetId="2" r:id="rId1"/>
+    <sheet name="akiApcMini2" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="83">
   <si>
     <t>Set</t>
   </si>
@@ -232,16 +233,73 @@
   </si>
   <si>
     <t>FULL</t>
+  </si>
+  <si>
+    <t>X1</t>
+  </si>
+  <si>
+    <t>X2</t>
+  </si>
+  <si>
+    <t>X3</t>
+  </si>
+  <si>
+    <t>X4</t>
+  </si>
+  <si>
+    <t>X5</t>
+  </si>
+  <si>
+    <t>X6</t>
+  </si>
+  <si>
+    <t>X7</t>
+  </si>
+  <si>
+    <t>X8</t>
+  </si>
+  <si>
+    <t>X9</t>
+  </si>
+  <si>
+    <t>X10</t>
+  </si>
+  <si>
+    <t>X11</t>
+  </si>
+  <si>
+    <t>X12</t>
+  </si>
+  <si>
+    <t>X13</t>
+  </si>
+  <si>
+    <t>X14</t>
+  </si>
+  <si>
+    <t>X15</t>
+  </si>
+  <si>
+    <t>X16</t>
+  </si>
+  <si>
+    <t>Store</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -647,6 +705,1115 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A5DA94-3567-451E-9067-A9BCE5CF7F57}">
+  <dimension ref="B1:K113"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="8">
+        <v>410</v>
+      </c>
+      <c r="C4" s="8">
+        <v>411</v>
+      </c>
+      <c r="D4" s="8">
+        <v>412</v>
+      </c>
+      <c r="E4" s="8">
+        <v>413</v>
+      </c>
+      <c r="F4" s="8">
+        <v>414</v>
+      </c>
+      <c r="G4" s="8">
+        <v>415</v>
+      </c>
+      <c r="H4" s="8">
+        <v>416</v>
+      </c>
+      <c r="I4" s="8">
+        <v>417</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="8">
+        <v>310</v>
+      </c>
+      <c r="C5" s="8">
+        <v>311</v>
+      </c>
+      <c r="D5" s="8">
+        <v>312</v>
+      </c>
+      <c r="E5" s="8">
+        <v>313</v>
+      </c>
+      <c r="F5" s="8">
+        <v>314</v>
+      </c>
+      <c r="G5" s="8">
+        <v>315</v>
+      </c>
+      <c r="H5" s="8">
+        <v>316</v>
+      </c>
+      <c r="I5" s="8">
+        <v>317</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="8">
+        <v>210</v>
+      </c>
+      <c r="C6" s="8">
+        <v>211</v>
+      </c>
+      <c r="D6" s="8">
+        <v>212</v>
+      </c>
+      <c r="E6" s="8">
+        <v>213</v>
+      </c>
+      <c r="F6" s="8">
+        <v>214</v>
+      </c>
+      <c r="G6" s="8">
+        <v>215</v>
+      </c>
+      <c r="H6" s="8">
+        <v>216</v>
+      </c>
+      <c r="I6" s="8">
+        <v>217</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="8">
+        <v>110</v>
+      </c>
+      <c r="C7" s="8">
+        <v>111</v>
+      </c>
+      <c r="D7" s="8">
+        <v>112</v>
+      </c>
+      <c r="E7" s="8">
+        <v>113</v>
+      </c>
+      <c r="F7" s="8">
+        <v>114</v>
+      </c>
+      <c r="G7" s="8">
+        <v>115</v>
+      </c>
+      <c r="H7" s="8">
+        <v>116</v>
+      </c>
+      <c r="I7" s="8">
+        <v>117</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="6">
+        <v>401</v>
+      </c>
+      <c r="C8" s="6">
+        <v>402</v>
+      </c>
+      <c r="D8" s="6">
+        <v>403</v>
+      </c>
+      <c r="E8" s="6">
+        <v>404</v>
+      </c>
+      <c r="F8" s="6">
+        <v>405</v>
+      </c>
+      <c r="G8" s="6">
+        <v>406</v>
+      </c>
+      <c r="H8" s="6">
+        <v>407</v>
+      </c>
+      <c r="I8" s="6">
+        <v>408</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="6">
+        <v>301</v>
+      </c>
+      <c r="C9" s="6">
+        <v>302</v>
+      </c>
+      <c r="D9" s="6">
+        <v>303</v>
+      </c>
+      <c r="E9" s="6">
+        <v>304</v>
+      </c>
+      <c r="F9" s="6">
+        <v>305</v>
+      </c>
+      <c r="G9" s="6">
+        <v>306</v>
+      </c>
+      <c r="H9" s="6">
+        <v>307</v>
+      </c>
+      <c r="I9" s="6">
+        <v>308</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="6">
+        <v>201</v>
+      </c>
+      <c r="C11" s="6">
+        <v>202</v>
+      </c>
+      <c r="D11" s="6">
+        <v>203</v>
+      </c>
+      <c r="E11" s="6">
+        <v>204</v>
+      </c>
+      <c r="F11" s="6">
+        <v>205</v>
+      </c>
+      <c r="G11" s="6">
+        <v>206</v>
+      </c>
+      <c r="H11" s="6">
+        <v>207</v>
+      </c>
+      <c r="I11" s="6">
+        <v>208</v>
+      </c>
+      <c r="K11" s="6">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:11" ht="184" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="6">
+        <v>201</v>
+      </c>
+      <c r="C13" s="6">
+        <v>202</v>
+      </c>
+      <c r="D13" s="6">
+        <v>203</v>
+      </c>
+      <c r="E13" s="6">
+        <v>204</v>
+      </c>
+      <c r="F13" s="6">
+        <v>205</v>
+      </c>
+      <c r="G13" s="6">
+        <v>206</v>
+      </c>
+      <c r="H13" s="6">
+        <v>207</v>
+      </c>
+      <c r="I13" s="6">
+        <v>208</v>
+      </c>
+      <c r="K13" s="6">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <f>B9</f>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f>C9</f>
+        <v>302</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <f>D9</f>
+        <v>303</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <f>E9</f>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <f>F9</f>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24">
+        <f>G9</f>
+        <v>306</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>6</v>
+      </c>
+      <c r="C25">
+        <f>H9</f>
+        <v>307</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="C26">
+        <f>I9</f>
+        <v>308</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="C27">
+        <f>B8</f>
+        <v>401</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <f>C8</f>
+        <v>402</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <f>D8</f>
+        <v>403</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>11</v>
+      </c>
+      <c r="C30">
+        <f>E8</f>
+        <v>404</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <f>F8</f>
+        <v>405</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>13</v>
+      </c>
+      <c r="C32">
+        <f>G8</f>
+        <v>406</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <f>H8</f>
+        <v>407</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <f>I8</f>
+        <v>408</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>16</v>
+      </c>
+      <c r="C35">
+        <f>B7</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <f>C7</f>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>18</v>
+      </c>
+      <c r="C37">
+        <f>D7</f>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>19</v>
+      </c>
+      <c r="C38">
+        <f>E7</f>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>20</v>
+      </c>
+      <c r="C39">
+        <f>F7</f>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>21</v>
+      </c>
+      <c r="C40">
+        <f>G7</f>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>22</v>
+      </c>
+      <c r="C41">
+        <f>H7</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>23</v>
+      </c>
+      <c r="C42">
+        <f>I7</f>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>24</v>
+      </c>
+      <c r="C43">
+        <f>B6</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>25</v>
+      </c>
+      <c r="C44">
+        <f>C6</f>
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>26</v>
+      </c>
+      <c r="C45">
+        <f>D6</f>
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>27</v>
+      </c>
+      <c r="C46">
+        <f>E6</f>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>28</v>
+      </c>
+      <c r="C47">
+        <f>F6</f>
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>29</v>
+      </c>
+      <c r="C48">
+        <f>G6</f>
+        <v>215</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>30</v>
+      </c>
+      <c r="C49">
+        <f>H6</f>
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>31</v>
+      </c>
+      <c r="C50">
+        <f>I6</f>
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>32</v>
+      </c>
+      <c r="C51">
+        <f>B5</f>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>33</v>
+      </c>
+      <c r="C52">
+        <f>C5</f>
+        <v>311</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>34</v>
+      </c>
+      <c r="C53">
+        <f>D5</f>
+        <v>312</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>35</v>
+      </c>
+      <c r="C54">
+        <f>E5</f>
+        <v>313</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>36</v>
+      </c>
+      <c r="C55">
+        <f>F5</f>
+        <v>314</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>37</v>
+      </c>
+      <c r="C56">
+        <f>G5</f>
+        <v>315</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>38</v>
+      </c>
+      <c r="C57">
+        <f>H5</f>
+        <v>316</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>39</v>
+      </c>
+      <c r="C58">
+        <f>I5</f>
+        <v>317</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>40</v>
+      </c>
+      <c r="C59">
+        <f>B4</f>
+        <v>410</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>41</v>
+      </c>
+      <c r="C60">
+        <f>C4</f>
+        <v>411</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>42</v>
+      </c>
+      <c r="C61">
+        <f>D4</f>
+        <v>412</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>43</v>
+      </c>
+      <c r="C62">
+        <f>E4</f>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>44</v>
+      </c>
+      <c r="C63">
+        <f>F4</f>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>45</v>
+      </c>
+      <c r="C64">
+        <f>G4</f>
+        <v>415</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>46</v>
+      </c>
+      <c r="C65">
+        <f>H4</f>
+        <v>416</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>47</v>
+      </c>
+      <c r="C66">
+        <f>I4</f>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>48</v>
+      </c>
+      <c r="C67" t="str">
+        <f>B3</f>
+        <v>X9</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>49</v>
+      </c>
+      <c r="C68" t="str">
+        <f>C3</f>
+        <v>X10</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>50</v>
+      </c>
+      <c r="C69" t="str">
+        <f>D3</f>
+        <v>X11</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>51</v>
+      </c>
+      <c r="C70" t="str">
+        <f>E3</f>
+        <v>X12</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>52</v>
+      </c>
+      <c r="C71" t="str">
+        <f>F3</f>
+        <v>X13</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>53</v>
+      </c>
+      <c r="C72" t="str">
+        <f>G3</f>
+        <v>X14</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>54</v>
+      </c>
+      <c r="C73" t="str">
+        <f>H3</f>
+        <v>X15</v>
+      </c>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>55</v>
+      </c>
+      <c r="C74" t="str">
+        <f>I3</f>
+        <v>X16</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>56</v>
+      </c>
+      <c r="C75" t="str">
+        <f>B2</f>
+        <v>X1</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>57</v>
+      </c>
+      <c r="C76" t="str">
+        <f>C2</f>
+        <v>X2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>58</v>
+      </c>
+      <c r="C77" t="str">
+        <f>D2</f>
+        <v>X3</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>59</v>
+      </c>
+      <c r="C78" t="str">
+        <f>E2</f>
+        <v>X4</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>60</v>
+      </c>
+      <c r="C79" t="str">
+        <f>F2</f>
+        <v>X5</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>61</v>
+      </c>
+      <c r="C80" t="str">
+        <f>G2</f>
+        <v>X6</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>62</v>
+      </c>
+      <c r="C81" t="str">
+        <f>H2</f>
+        <v>X7</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>63</v>
+      </c>
+      <c r="C82" t="str">
+        <f>I2</f>
+        <v>X8</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <v>64</v>
+      </c>
+      <c r="C83">
+        <f>B11</f>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>65</v>
+      </c>
+      <c r="C84">
+        <f>C11</f>
+        <v>202</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>66</v>
+      </c>
+      <c r="C85">
+        <f>D11</f>
+        <v>203</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>67</v>
+      </c>
+      <c r="C86">
+        <f>E11</f>
+        <v>204</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>68</v>
+      </c>
+      <c r="C87">
+        <f>F11</f>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B88">
+        <v>69</v>
+      </c>
+      <c r="C88">
+        <f>G11</f>
+        <v>206</v>
+      </c>
+    </row>
+    <row r="89" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B89">
+        <v>70</v>
+      </c>
+      <c r="C89">
+        <f>H11</f>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B90">
+        <v>71</v>
+      </c>
+      <c r="C90">
+        <f>I11</f>
+        <v>208</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B91">
+        <v>72</v>
+      </c>
+      <c r="C91">
+        <f>K11</f>
+        <v>209</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B92">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B93">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B94">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B95">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B96">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B97">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B98">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B99">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B100">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B101">
+        <v>82</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" ref="C101:C105" si="0">K2</f>
+        <v>ESC</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B102">
+        <v>83</v>
+      </c>
+      <c r="C102" t="str">
+        <f t="shared" si="0"/>
+        <v>CLEAR</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B103">
+        <v>84</v>
+      </c>
+      <c r="C103" t="str">
+        <f t="shared" si="0"/>
+        <v>Store</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B104">
+        <v>85</v>
+      </c>
+      <c r="C104" t="str">
+        <f t="shared" si="0"/>
+        <v>HIGHLIGHT</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B105">
+        <v>86</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="0"/>
+        <v>BLIND</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B106">
+        <v>87</v>
+      </c>
+      <c r="C106" t="str">
+        <f>K7</f>
+        <v>MOVE</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B107">
+        <v>88</v>
+      </c>
+      <c r="C107" t="str">
+        <f>K8</f>
+        <v>FULL</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B108">
+        <v>89</v>
+      </c>
+      <c r="C108" t="str">
+        <f>K9</f>
+        <v>OOPS</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B109">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B110">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="111" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B111">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="112" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B112">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B113">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA8DEA62-A6EE-4460-B6E7-D1406ADBE8A9}">
   <dimension ref="B1:K113"/>
   <sheetViews>
@@ -654,7 +1821,7 @@
       <pane xSplit="1" ySplit="14" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1612,7 +2779,7 @@
         <v>82</v>
       </c>
       <c r="C101" t="str">
-        <f>K2</f>
+        <f t="shared" ref="C101:C108" si="0">K2</f>
         <v>ESC</v>
       </c>
     </row>
@@ -1621,7 +2788,7 @@
         <v>83</v>
       </c>
       <c r="C102" t="str">
-        <f>K3</f>
+        <f t="shared" si="0"/>
         <v>CLEAR</v>
       </c>
     </row>
@@ -1630,7 +2797,7 @@
         <v>84</v>
       </c>
       <c r="C103" t="str">
-        <f>K4</f>
+        <f t="shared" si="0"/>
         <v>XKEYS</v>
       </c>
     </row>
@@ -1639,7 +2806,7 @@
         <v>85</v>
       </c>
       <c r="C104" t="str">
-        <f>K5</f>
+        <f t="shared" si="0"/>
         <v>LIST</v>
       </c>
     </row>
@@ -1648,7 +2815,7 @@
         <v>86</v>
       </c>
       <c r="C105" t="str">
-        <f>K6</f>
+        <f t="shared" si="0"/>
         <v>MENU</v>
       </c>
     </row>
@@ -1657,7 +2824,7 @@
         <v>87</v>
       </c>
       <c r="C106">
-        <f>K7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1666,7 +2833,7 @@
         <v>88</v>
       </c>
       <c r="C107" t="str">
-        <f>K8</f>
+        <f t="shared" si="0"/>
         <v>OOPS</v>
       </c>
     </row>
@@ -1675,7 +2842,7 @@
         <v>89</v>
       </c>
       <c r="C108" t="str">
-        <f>K9</f>
+        <f t="shared" si="0"/>
         <v>FULL</v>
       </c>
     </row>

</xml_diff>